<commit_message>
Tests pass. Still need to do cleanup.
</commit_message>
<xml_diff>
--- a/data/formatted_writable_set_style.xlsx
+++ b/data/formatted_writable_set_style.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Total Sales</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>East</t>
+  </si>
+  <si>
+    <t>$ CHG</t>
   </si>
 </sst>
 </file>
@@ -599,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DD21AA-BB42-4B93-A906-23786677C348}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -616,22 +619,22 @@
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s" s="1">
         <v>8</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>0</v>
       </c>
       <c r="C4" s="5"/>
@@ -640,53 +643,102 @@
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" t="s" s="9">
         <v>3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" t="s" s="9">
         <v>4</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="E5" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" t="s" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="str">
+    <row r="6" spans="1:7">
+      <c r="A6" t="str" s="12">
         <f>A1</f>
         <v>East</v>
       </c>
       <c r="B6" s="13">
+        <v>750</v>
+      </c>
+      <c r="C6" s="14">
         <v>500</v>
       </c>
-      <c r="C6" s="14">
-        <v>400</v>
-      </c>
       <c r="D6" s="14">
-        <v>300</v>
+        <v>440</v>
       </c>
       <c r="E6" s="14">
-        <f>B6-C6</f>
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="F6" s="15">
-        <f>E6/C6</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="16">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="13">
+        <v>500</v>
+      </c>
+      <c r="C7" s="14">
+        <v>640</v>
+      </c>
+      <c r="D7" s="14">
+        <v>470</v>
+      </c>
+      <c r="E7" s="14">
+        <v>-140</v>
+      </c>
+      <c r="F7" s="15">
+        <v>-0.21875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="13">
+        <v>600</v>
+      </c>
+      <c r="C8" s="14">
+        <v>500</v>
+      </c>
+      <c r="D8" s="14">
+        <v>450</v>
+      </c>
+      <c r="E8" s="14">
+        <v>100</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="13">
+        <v>400</v>
+      </c>
+      <c r="C9" s="14">
+        <v>800</v>
+      </c>
+      <c r="D9" s="14">
+        <v>310</v>
+      </c>
+      <c r="E9" s="14">
+        <v>-400</v>
+      </c>
+      <c r="F9" s="15">
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up and tests pass. Moving on for now.
</commit_message>
<xml_diff>
--- a/data/formatted_writable_set_style.xlsx
+++ b/data/formatted_writable_set_style.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Total Sales</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>East</t>
-  </si>
-  <si>
-    <t>$ CHG</t>
   </si>
 </sst>
 </file>
@@ -602,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DD21AA-BB42-4B93-A906-23786677C348}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -619,22 +616,22 @@
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5"/>
@@ -643,102 +640,53 @@
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s" s="8">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s" s="9">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s" s="9">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s" s="9">
+      <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s" s="10">
+      <c r="E5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s" s="11">
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="str" s="12">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="str">
         <f>A1</f>
         <v>East</v>
       </c>
       <c r="B6" s="13">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="C6" s="14">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D6" s="14">
-        <v>440</v>
+        <v>300</v>
       </c>
       <c r="E6" s="14">
-        <v>250</v>
+        <f>B6-C6</f>
+        <v>100</v>
       </c>
       <c r="F6" s="15">
-        <v>0.5</v>
+        <f>E6/C6</f>
+        <v>0.25</v>
       </c>
       <c r="G6" s="16">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="13">
-        <v>500</v>
-      </c>
-      <c r="C7" s="14">
-        <v>640</v>
-      </c>
-      <c r="D7" s="14">
-        <v>470</v>
-      </c>
-      <c r="E7" s="14">
-        <v>-140</v>
-      </c>
-      <c r="F7" s="15">
-        <v>-0.21875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="13">
-        <v>600</v>
-      </c>
-      <c r="C8" s="14">
-        <v>500</v>
-      </c>
-      <c r="D8" s="14">
-        <v>450</v>
-      </c>
-      <c r="E8" s="14">
-        <v>100</v>
-      </c>
-      <c r="F8" s="15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="13">
-        <v>400</v>
-      </c>
-      <c r="C9" s="14">
-        <v>800</v>
-      </c>
-      <c r="D9" s="14">
-        <v>310</v>
-      </c>
-      <c r="E9" s="14">
-        <v>-400</v>
-      </c>
-      <c r="F9" s="15">
-        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>